<commit_message>
Fix detail of stock-check request
</commit_message>
<xml_diff>
--- a/src/assets/export-templates/template_xuat_ban.xlsx
+++ b/src/assets/export-templates/template_xuat_ban.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\export-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A56F72E-0224-49A9-9D67-FF54C36B1003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858E9423-77C8-4881-9FA9-7F1B5E2489D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9FA52C3A-7928-408F-877C-18AC7D4D703A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{9FA52C3A-7928-408F-877C-18AC7D4D703A}"/>
   </bookViews>
   <sheets>
     <sheet name="Template xuất bán" sheetId="2" r:id="rId1"/>
+    <sheet name="Bảng đơn vị" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Loại xuất</t>
   </si>
@@ -70,12 +71,42 @@
   <si>
     <t>Số lượng cần xuất</t>
   </si>
+  <si>
+    <t>Đơn vị tính</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>unit_type</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>KHO</t>
+  </si>
+  <si>
+    <t>NUT</t>
+  </si>
+  <si>
+    <t>VAI</t>
+  </si>
+  <si>
+    <t>Cuộn</t>
+  </si>
+  <si>
+    <t>Bịch</t>
+  </si>
+  <si>
+    <t>Cây</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,8 +141,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,8 +163,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -241,11 +286,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -282,11 +417,68 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -684,48 +876,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6856CC1-CBFE-4ECB-B377-3A86D1DC5596}">
-  <dimension ref="A1:C201"/>
+  <dimension ref="A1:D201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.26953125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="40.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.90625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="9" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="9" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10"/>
       <c r="B1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="14"/>
     </row>
-    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="14"/>
     </row>
-    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="C3" s="14"/>
     </row>
-    <row r="4" spans="1:3" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="10"/>
       <c r="B4" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="14"/>
     </row>
-    <row r="5" spans="1:3" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10"/>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
@@ -734,35 +927,35 @@
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="C11" s="14"/>
     </row>
-    <row r="12" spans="1:3" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
@@ -772,1146 +965,1911 @@
       <c r="C12" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="str">
         <f>IF(B13&lt;&gt;"", COUNTA($B$13:B13), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B13,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="str">
         <f>IF(B14&lt;&gt;"", COUNTA($B$13:B14), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B14,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="str">
         <f>IF(B15&lt;&gt;"", COUNTA($B$13:B15), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B15,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="str">
         <f>IF(B16&lt;&gt;"", COUNTA($B$13:B16), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B16,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="str">
         <f>IF(B17&lt;&gt;"", COUNTA($B$13:B17), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B17,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="str">
         <f>IF(B18&lt;&gt;"", COUNTA($B$13:B18), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B18,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="str">
         <f>IF(B19&lt;&gt;"", COUNTA($B$13:B19), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B19,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="str">
         <f>IF(B20&lt;&gt;"", COUNTA($B$13:B20), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B20,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="str">
         <f>IF(B21&lt;&gt;"", COUNTA($B$13:B21), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B21,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="str">
         <f>IF(B22&lt;&gt;"", COUNTA($B$13:B22), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B22,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="str">
         <f>IF(B23&lt;&gt;"", COUNTA($B$13:B23), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B23,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="str">
         <f>IF(B24&lt;&gt;"", COUNTA($B$13:B24), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B24,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="str">
         <f>IF(B25&lt;&gt;"", COUNTA($B$13:B25), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D25" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B25,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="str">
         <f>IF(B26&lt;&gt;"", COUNTA($B$13:B26), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D26" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B26,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="str">
         <f>IF(B27&lt;&gt;"", COUNTA($B$13:B27), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B27,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="str">
         <f>IF(B28&lt;&gt;"", COUNTA($B$13:B28), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B28,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="str">
         <f>IF(B29&lt;&gt;"", COUNTA($B$13:B29), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B29,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="str">
         <f>IF(B30&lt;&gt;"", COUNTA($B$13:B30), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B30,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="str">
         <f>IF(B31&lt;&gt;"", COUNTA($B$13:B31), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B31,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="str">
         <f>IF(B32&lt;&gt;"", COUNTA($B$13:B32), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B32,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="str">
         <f>IF(B33&lt;&gt;"", COUNTA($B$13:B33), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B33,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="str">
         <f>IF(B34&lt;&gt;"", COUNTA($B$13:B34), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B34,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="str">
         <f>IF(B35&lt;&gt;"", COUNTA($B$13:B35), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B35,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="str">
         <f>IF(B36&lt;&gt;"", COUNTA($B$13:B36), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B36,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="str">
         <f>IF(B37&lt;&gt;"", COUNTA($B$13:B37), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B37,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="str">
         <f>IF(B38&lt;&gt;"", COUNTA($B$13:B38), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B38,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="str">
         <f>IF(B39&lt;&gt;"", COUNTA($B$13:B39), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B39,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="str">
         <f>IF(B40&lt;&gt;"", COUNTA($B$13:B40), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B40,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="str">
         <f>IF(B41&lt;&gt;"", COUNTA($B$13:B41), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B41,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="str">
         <f>IF(B42&lt;&gt;"", COUNTA($B$13:B42), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B42,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="str">
         <f>IF(B43&lt;&gt;"", COUNTA($B$13:B43), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B43,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="str">
         <f>IF(B44&lt;&gt;"", COUNTA($B$13:B44), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B44,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="str">
         <f>IF(B45&lt;&gt;"", COUNTA($B$13:B45), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B45,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="str">
         <f>IF(B46&lt;&gt;"", COUNTA($B$13:B46), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B46,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="str">
         <f>IF(B47&lt;&gt;"", COUNTA($B$13:B47), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B47,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="str">
         <f>IF(B48&lt;&gt;"", COUNTA($B$13:B48), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B48,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="str">
         <f>IF(B49&lt;&gt;"", COUNTA($B$13:B49), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B49,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="str">
         <f>IF(B50&lt;&gt;"", COUNTA($B$13:B50), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B50,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="10" t="str">
         <f>IF(B51&lt;&gt;"", COUNTA($B$13:B51), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B51,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="10" t="str">
         <f>IF(B52&lt;&gt;"", COUNTA($B$13:B52), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D52" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B52,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="str">
         <f>IF(B53&lt;&gt;"", COUNTA($B$13:B53), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B53,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="10" t="str">
         <f>IF(B54&lt;&gt;"", COUNTA($B$13:B54), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B54,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="str">
         <f>IF(B55&lt;&gt;"", COUNTA($B$13:B55), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B55,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="str">
         <f>IF(B56&lt;&gt;"", COUNTA($B$13:B56), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D56" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B56,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="str">
         <f>IF(B57&lt;&gt;"", COUNTA($B$13:B57), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D57" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B57,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="str">
         <f>IF(B58&lt;&gt;"", COUNTA($B$13:B58), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D58" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B58,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="str">
         <f>IF(B59&lt;&gt;"", COUNTA($B$13:B59), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D59" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B59,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="10" t="str">
         <f>IF(B60&lt;&gt;"", COUNTA($B$13:B60), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D60" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B60,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="str">
         <f>IF(B61&lt;&gt;"", COUNTA($B$13:B61), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D61" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B61,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="str">
         <f>IF(B62&lt;&gt;"", COUNTA($B$13:B62), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D62" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B62,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="10" t="str">
         <f>IF(B63&lt;&gt;"", COUNTA($B$13:B63), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D63" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B63,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="str">
         <f>IF(B64&lt;&gt;"", COUNTA($B$13:B64), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D64" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B64,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="str">
         <f>IF(B65&lt;&gt;"", COUNTA($B$13:B65), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D65" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B65,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="str">
         <f>IF(B66&lt;&gt;"", COUNTA($B$13:B66), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D66" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B66,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="10" t="str">
         <f>IF(B67&lt;&gt;"", COUNTA($B$13:B67), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D67" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B67,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="str">
         <f>IF(B68&lt;&gt;"", COUNTA($B$13:B68), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D68" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B68,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="str">
         <f>IF(B69&lt;&gt;"", COUNTA($B$13:B69), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D69" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B69,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="str">
         <f>IF(B70&lt;&gt;"", COUNTA($B$13:B70), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D70" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B70,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="str">
         <f>IF(B71&lt;&gt;"", COUNTA($B$13:B71), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D71" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B71,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="str">
         <f>IF(B72&lt;&gt;"", COUNTA($B$13:B72), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D72" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B72,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="10" t="str">
         <f>IF(B73&lt;&gt;"", COUNTA($B$13:B73), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D73" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B73,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="str">
         <f>IF(B74&lt;&gt;"", COUNTA($B$13:B74), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D74" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B74,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="str">
         <f>IF(B75&lt;&gt;"", COUNTA($B$13:B75), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D75" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B75,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="str">
         <f>IF(B76&lt;&gt;"", COUNTA($B$13:B76), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D76" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B76,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="10" t="str">
         <f>IF(B77&lt;&gt;"", COUNTA($B$13:B77), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D77" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B77,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="10" t="str">
         <f>IF(B78&lt;&gt;"", COUNTA($B$13:B78), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D78" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B78,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="10" t="str">
         <f>IF(B79&lt;&gt;"", COUNTA($B$13:B79), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D79" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B79,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="10" t="str">
         <f>IF(B80&lt;&gt;"", COUNTA($B$13:B80), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D80" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B80,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="10" t="str">
         <f>IF(B81&lt;&gt;"", COUNTA($B$13:B81), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D81" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B81,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="10" t="str">
         <f>IF(B82&lt;&gt;"", COUNTA($B$13:B82), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D82" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B82,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="10" t="str">
         <f>IF(B83&lt;&gt;"", COUNTA($B$13:B83), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D83" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B83,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="10" t="str">
         <f>IF(B84&lt;&gt;"", COUNTA($B$13:B84), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D84" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B84,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="10" t="str">
         <f>IF(B85&lt;&gt;"", COUNTA($B$13:B85), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D85" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B85,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="10" t="str">
         <f>IF(B86&lt;&gt;"", COUNTA($B$13:B86), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D86" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B86,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="10" t="str">
         <f>IF(B87&lt;&gt;"", COUNTA($B$13:B87), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D87" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B87,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="10" t="str">
         <f>IF(B88&lt;&gt;"", COUNTA($B$13:B88), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D88" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B88,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="10" t="str">
         <f>IF(B89&lt;&gt;"", COUNTA($B$13:B89), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D89" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B89,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="10" t="str">
         <f>IF(B90&lt;&gt;"", COUNTA($B$13:B90), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D90" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B90,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="10" t="str">
         <f>IF(B91&lt;&gt;"", COUNTA($B$13:B91), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D91" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B91,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="10" t="str">
         <f>IF(B92&lt;&gt;"", COUNTA($B$13:B92), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D92" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B92,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="10" t="str">
         <f>IF(B93&lt;&gt;"", COUNTA($B$13:B93), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D93" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B93,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="10" t="str">
         <f>IF(B94&lt;&gt;"", COUNTA($B$13:B94), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D94" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B94,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="10" t="str">
         <f>IF(B95&lt;&gt;"", COUNTA($B$13:B95), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D95" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B95,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="10" t="str">
         <f>IF(B96&lt;&gt;"", COUNTA($B$13:B96), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D96" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B96,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="10" t="str">
         <f>IF(B97&lt;&gt;"", COUNTA($B$13:B97), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D97" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B97,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="10" t="str">
         <f>IF(B98&lt;&gt;"", COUNTA($B$13:B98), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D98" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B98,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="10" t="str">
         <f>IF(B99&lt;&gt;"", COUNTA($B$13:B99), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D99" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B99,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="10" t="str">
         <f>IF(B100&lt;&gt;"", COUNTA($B$13:B100), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D100" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B100,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="10" t="str">
         <f>IF(B101&lt;&gt;"", COUNTA($B$13:B101), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D101" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B101,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="10" t="str">
         <f>IF(B102&lt;&gt;"", COUNTA($B$13:B102), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D102" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B102,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="10" t="str">
         <f>IF(B103&lt;&gt;"", COUNTA($B$13:B103), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D103" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B103,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="10" t="str">
         <f>IF(B104&lt;&gt;"", COUNTA($B$13:B104), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D104" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B104,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="10" t="str">
         <f>IF(B105&lt;&gt;"", COUNTA($B$13:B105), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D105" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B105,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="10" t="str">
         <f>IF(B106&lt;&gt;"", COUNTA($B$13:B106), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D106" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B106,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="10" t="str">
         <f>IF(B107&lt;&gt;"", COUNTA($B$13:B107), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D107" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B107,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="10" t="str">
         <f>IF(B108&lt;&gt;"", COUNTA($B$13:B108), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D108" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B108,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="10" t="str">
         <f>IF(B109&lt;&gt;"", COUNTA($B$13:B109), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D109" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B109,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="10" t="str">
         <f>IF(B110&lt;&gt;"", COUNTA($B$13:B110), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D110" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B110,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="10" t="str">
         <f>IF(B111&lt;&gt;"", COUNTA($B$13:B111), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D111" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B111,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="10" t="str">
         <f>IF(B112&lt;&gt;"", COUNTA($B$13:B112), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D112" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B112,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="10" t="str">
         <f>IF(B113&lt;&gt;"", COUNTA($B$13:B113), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D113" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B113,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="10" t="str">
         <f>IF(B114&lt;&gt;"", COUNTA($B$13:B114), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D114" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B114,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="10" t="str">
         <f>IF(B115&lt;&gt;"", COUNTA($B$13:B115), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D115" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B115,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="10" t="str">
         <f>IF(B116&lt;&gt;"", COUNTA($B$13:B116), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D116" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B116,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="10" t="str">
         <f>IF(B117&lt;&gt;"", COUNTA($B$13:B117), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D117" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B117,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="10" t="str">
         <f>IF(B118&lt;&gt;"", COUNTA($B$13:B118), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D118" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B118,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="10" t="str">
         <f>IF(B119&lt;&gt;"", COUNTA($B$13:B119), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D119" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B119,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="10" t="str">
         <f>IF(B120&lt;&gt;"", COUNTA($B$13:B120), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D120" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B120,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="10" t="str">
         <f>IF(B121&lt;&gt;"", COUNTA($B$13:B121), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D121" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B121,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" s="10" t="str">
         <f>IF(B122&lt;&gt;"", COUNTA($B$13:B122), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D122" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B122,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="10" t="str">
         <f>IF(B123&lt;&gt;"", COUNTA($B$13:B123), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D123" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B123,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="10" t="str">
         <f>IF(B124&lt;&gt;"", COUNTA($B$13:B124), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D124" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B124,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" s="10" t="str">
         <f>IF(B125&lt;&gt;"", COUNTA($B$13:B125), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D125" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B125,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="10" t="str">
         <f>IF(B126&lt;&gt;"", COUNTA($B$13:B126), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D126" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B126,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" s="10" t="str">
         <f>IF(B127&lt;&gt;"", COUNTA($B$13:B127), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D127" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B127,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" s="10" t="str">
         <f>IF(B128&lt;&gt;"", COUNTA($B$13:B128), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D128" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B128,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" s="10" t="str">
         <f>IF(B129&lt;&gt;"", COUNTA($B$13:B129), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D129" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B129,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" s="10" t="str">
         <f>IF(B130&lt;&gt;"", COUNTA($B$13:B130), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D130" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B130,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" s="10" t="str">
         <f>IF(B131&lt;&gt;"", COUNTA($B$13:B131), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D131" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B131,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" s="10" t="str">
         <f>IF(B132&lt;&gt;"", COUNTA($B$13:B132), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D132" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B132,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="10" t="str">
         <f>IF(B133&lt;&gt;"", COUNTA($B$13:B133), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D133" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B133,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" s="10" t="str">
         <f>IF(B134&lt;&gt;"", COUNTA($B$13:B134), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D134" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B134,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" s="10" t="str">
         <f>IF(B135&lt;&gt;"", COUNTA($B$13:B135), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D135" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B135,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" s="10" t="str">
         <f>IF(B136&lt;&gt;"", COUNTA($B$13:B136), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D136" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B136,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" s="10" t="str">
         <f>IF(B137&lt;&gt;"", COUNTA($B$13:B137), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D137" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B137,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" s="10" t="str">
         <f>IF(B138&lt;&gt;"", COUNTA($B$13:B138), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D138" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B138,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" s="10" t="str">
         <f>IF(B139&lt;&gt;"", COUNTA($B$13:B139), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D139" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B139,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" s="10" t="str">
         <f>IF(B140&lt;&gt;"", COUNTA($B$13:B140), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D140" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B140,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" s="10" t="str">
         <f>IF(B141&lt;&gt;"", COUNTA($B$13:B141), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D141" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B141,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" s="10" t="str">
         <f>IF(B142&lt;&gt;"", COUNTA($B$13:B142), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D142" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B142,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" s="10" t="str">
         <f>IF(B143&lt;&gt;"", COUNTA($B$13:B143), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D143" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B143,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" s="10" t="str">
         <f>IF(B144&lt;&gt;"", COUNTA($B$13:B144), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D144" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B144,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" s="10" t="str">
         <f>IF(B145&lt;&gt;"", COUNTA($B$13:B145), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D145" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B145,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" s="10" t="str">
         <f>IF(B146&lt;&gt;"", COUNTA($B$13:B146), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D146" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B146,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" s="10" t="str">
         <f>IF(B147&lt;&gt;"", COUNTA($B$13:B147), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D147" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B147,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" s="10" t="str">
         <f>IF(B148&lt;&gt;"", COUNTA($B$13:B148), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D148" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B148,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" s="10" t="str">
         <f>IF(B149&lt;&gt;"", COUNTA($B$13:B149), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D149" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B149,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" s="10" t="str">
         <f>IF(B150&lt;&gt;"", COUNTA($B$13:B150), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D150" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B150,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" s="10" t="str">
         <f>IF(B151&lt;&gt;"", COUNTA($B$13:B151), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D151" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B151,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" s="10" t="str">
         <f>IF(B152&lt;&gt;"", COUNTA($B$13:B152), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D152" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B152,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" s="10" t="str">
         <f>IF(B153&lt;&gt;"", COUNTA($B$13:B153), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D153" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B153,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" s="10" t="str">
         <f>IF(B154&lt;&gt;"", COUNTA($B$13:B154), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D154" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B154,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" s="10" t="str">
         <f>IF(B155&lt;&gt;"", COUNTA($B$13:B155), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D155" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B155,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" s="10" t="str">
         <f>IF(B156&lt;&gt;"", COUNTA($B$13:B156), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D156" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B156,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" s="10" t="str">
         <f>IF(B157&lt;&gt;"", COUNTA($B$13:B157), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D157" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B157,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" s="10" t="str">
         <f>IF(B158&lt;&gt;"", COUNTA($B$13:B158), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D158" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B158,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" s="10" t="str">
         <f>IF(B159&lt;&gt;"", COUNTA($B$13:B159), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D159" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B159,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" s="10" t="str">
         <f>IF(B160&lt;&gt;"", COUNTA($B$13:B160), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D160" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B160,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" s="10" t="str">
         <f>IF(B161&lt;&gt;"", COUNTA($B$13:B161), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D161" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B161,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" s="10" t="str">
         <f>IF(B162&lt;&gt;"", COUNTA($B$13:B162), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D162" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B162,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" s="10" t="str">
         <f>IF(B163&lt;&gt;"", COUNTA($B$13:B163), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D163" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B163,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" s="10" t="str">
         <f>IF(B164&lt;&gt;"", COUNTA($B$13:B164), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D164" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B164,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" s="10" t="str">
         <f>IF(B165&lt;&gt;"", COUNTA($B$13:B165), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D165" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B165,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" s="10" t="str">
         <f>IF(B166&lt;&gt;"", COUNTA($B$13:B166), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D166" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B166,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" s="10" t="str">
         <f>IF(B167&lt;&gt;"", COUNTA($B$13:B167), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D167" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B167,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" s="10" t="str">
         <f>IF(B168&lt;&gt;"", COUNTA($B$13:B168), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D168" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B168,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" s="10" t="str">
         <f>IF(B169&lt;&gt;"", COUNTA($B$13:B169), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D169" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B169,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" s="10" t="str">
         <f>IF(B170&lt;&gt;"", COUNTA($B$13:B170), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D170" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B170,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" s="10" t="str">
         <f>IF(B171&lt;&gt;"", COUNTA($B$13:B171), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D171" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B171,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" s="10" t="str">
         <f>IF(B172&lt;&gt;"", COUNTA($B$13:B172), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D172" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B172,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" s="10" t="str">
         <f>IF(B173&lt;&gt;"", COUNTA($B$13:B173), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D173" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B173,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" s="10" t="str">
         <f>IF(B174&lt;&gt;"", COUNTA($B$13:B174), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D174" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B174,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" s="10" t="str">
         <f>IF(B175&lt;&gt;"", COUNTA($B$13:B175), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D175" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B175,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" s="10" t="str">
         <f>IF(B176&lt;&gt;"", COUNTA($B$13:B176), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D176" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B176,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" s="10" t="str">
         <f>IF(B177&lt;&gt;"", COUNTA($B$13:B177), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D177" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B177,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" s="10" t="str">
         <f>IF(B178&lt;&gt;"", COUNTA($B$13:B178), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D178" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B178,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" s="10" t="str">
         <f>IF(B179&lt;&gt;"", COUNTA($B$13:B179), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D179" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B179,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" s="10" t="str">
         <f>IF(B180&lt;&gt;"", COUNTA($B$13:B180), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D180" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B180,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" s="10" t="str">
         <f>IF(B181&lt;&gt;"", COUNTA($B$13:B181), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D181" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B181,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" s="10" t="str">
         <f>IF(B182&lt;&gt;"", COUNTA($B$13:B182), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D182" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B182,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183" s="10" t="str">
         <f>IF(B183&lt;&gt;"", COUNTA($B$13:B183), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D183" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B183,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" s="10" t="str">
         <f>IF(B184&lt;&gt;"", COUNTA($B$13:B184), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D184" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B184,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" s="10" t="str">
         <f>IF(B185&lt;&gt;"", COUNTA($B$13:B185), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D185" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B185,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186" s="10" t="str">
         <f>IF(B186&lt;&gt;"", COUNTA($B$13:B186), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D186" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B186,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187" s="10" t="str">
         <f>IF(B187&lt;&gt;"", COUNTA($B$13:B187), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D187" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B187,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188" s="10" t="str">
         <f>IF(B188&lt;&gt;"", COUNTA($B$13:B188), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D188" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B188,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189" s="10" t="str">
         <f>IF(B189&lt;&gt;"", COUNTA($B$13:B189), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D189" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B189,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" s="10" t="str">
         <f>IF(B190&lt;&gt;"", COUNTA($B$13:B190), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D190" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B190,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191" s="10" t="str">
         <f>IF(B191&lt;&gt;"", COUNTA($B$13:B191), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D191" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B191,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" s="10" t="str">
         <f>IF(B192&lt;&gt;"", COUNTA($B$13:B192), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D192" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B192,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193" s="10" t="str">
         <f>IF(B193&lt;&gt;"", COUNTA($B$13:B193), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D193" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B193,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A194" s="10" t="str">
         <f>IF(B194&lt;&gt;"", COUNTA($B$13:B194), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D194" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B194,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" s="10" t="str">
         <f>IF(B195&lt;&gt;"", COUNTA($B$13:B195), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D195" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B195,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196" s="10" t="str">
         <f>IF(B196&lt;&gt;"", COUNTA($B$13:B196), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D196" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B196,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" s="10" t="str">
         <f>IF(B197&lt;&gt;"", COUNTA($B$13:B197), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D197" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B197,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198" s="10" t="str">
         <f>IF(B198&lt;&gt;"", COUNTA($B$13:B198), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D198" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B198,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199" s="10" t="str">
         <f>IF(B199&lt;&gt;"", COUNTA($B$13:B199), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D199" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B199,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200" s="10" t="str">
         <f>IF(B200&lt;&gt;"", COUNTA($B$13:B200), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D200" s="1" t="str">
+        <f>IFERROR(VLOOKUP(LEFT(B200,3),'Bảng đơn vị'!A:B,2,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" s="10" t="str">
         <f>IF(B201&lt;&gt;"", COUNTA($B$13:B201), "")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="y8Ncih9DW9Kgzraf7Rlczm0caWg0igRdOzOBqAdh8X5AnNJ5ryLGXS0k0SlhKeTKbFEcy+cn91TdJDD47Vd3ZQ==" saltValue="xfE7xm80n96qqFK4F+PkcQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FIKNBg53GW2hUHDy67pNfL/7jmZdCmKhoDVIZKhoaEDz4xLE/G3atHiqsL5OrO81Bt/5lkB1lpOeZ+nlMLHlYw==" saltValue="Bsm6aLSLbREpLplBB/Xu4w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="A12:C201">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>A12&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>D12&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D200">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>A12&lt;&gt;""</formula>
+      <formula>$B13&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -1922,4 +2880,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703C20E1-24F1-4490-998A-D5D50D717C36}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" style="17" customWidth="1"/>
+    <col min="3" max="16384" width="8.7265625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Pw/0F6v/nXKFmaKeN445PjRtPNBfttR80pt7Wi5x1cEWh1HbMldvuKv10kkWm6I0ko2vbiR1a7aMbaE4qwE/FQ==" saltValue="HDnwqizx0vyAtwpGEu2uTg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>